<commit_message>
medicine choices, assistant,change regno and date
</commit_message>
<xml_diff>
--- a/app/config/tables/MADTRIAL_INC/Forms/MADTRIAL_INC/MADTRIAL_INC.xlsx
+++ b/app/config/tables/MADTRIAL_INC/Forms/MADTRIAL_INC/MADTRIAL_INC.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C35A8E5-790C-4F86-AF2A-25D70BCF7AE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F6271-5A4F-4747-99AC-39743E9A3ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="484">
   <si>
     <t>setting_name</t>
   </si>
@@ -1305,139 +1305,199 @@
     <t>data('BAIRRO') != 77</t>
   </si>
   <si>
+    <t>data('CAMOONDE') != null || data('TABZ') == 7777 || data('CAMO') != 9999</t>
+  </si>
+  <si>
+    <t>data('CAMO') != null || data('CAMOONDE') != null</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>Abrao</t>
+  </si>
+  <si>
+    <t>Augosto Da Costa</t>
+  </si>
+  <si>
+    <t>Abdel</t>
+  </si>
+  <si>
+    <t>Fatima</t>
+  </si>
+  <si>
+    <t>TRATAMENT_A</t>
+  </si>
+  <si>
+    <t>A criança recebeu algum tratamento (antes inclusao)?</t>
+  </si>
+  <si>
+    <t>data('TRATAMENT_A') =='1'</t>
+  </si>
+  <si>
+    <t>TRATQUAL_A</t>
+  </si>
+  <si>
+    <t>TRATAMENT_R</t>
+  </si>
+  <si>
+    <t>Did the child get any treatments prescribed?</t>
+  </si>
+  <si>
+    <t>A criança deve receber algum tratamento (receita)?</t>
+  </si>
+  <si>
+    <t>TRATQUAL_R</t>
+  </si>
+  <si>
+    <t>What treatments are prescribed ?</t>
+  </si>
+  <si>
+    <t>Qual tratamento foi receitado?</t>
+  </si>
+  <si>
+    <t>TRATQUALOU_R</t>
+  </si>
+  <si>
+    <t>TRATQUALOU_A</t>
+  </si>
+  <si>
+    <t>selected(data('TRATQUAL_R'),'77')</t>
+  </si>
+  <si>
+    <t>data('TRATAMENT_R') =='1'</t>
+  </si>
+  <si>
+    <t>selected(data('TRATQUAL_A'),'77')</t>
+  </si>
+  <si>
+    <t>Paracetamol</t>
+  </si>
+  <si>
+    <t>Amoxicillina</t>
+  </si>
+  <si>
+    <t>Complexo B</t>
+  </si>
+  <si>
+    <t>Salbutamol</t>
+  </si>
+  <si>
+    <t>Diazepam</t>
+  </si>
+  <si>
+    <t>Prometazina</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>removed Suzete (enf=1) on 19-01-2022</t>
+  </si>
+  <si>
+    <t>removed Suzete (ass=11) on 19-01-2022</t>
+  </si>
+  <si>
+    <t>Soro fisiologico</t>
+  </si>
+  <si>
+    <t>Vitamina C</t>
+  </si>
+  <si>
+    <t>SRO</t>
+  </si>
+  <si>
+    <t>Sulfate de Zinco</t>
+  </si>
+  <si>
+    <t>Azitomicina</t>
+  </si>
+  <si>
+    <t>Brufen</t>
+  </si>
+  <si>
+    <t>Albendazol</t>
+  </si>
+  <si>
+    <t>Mebendazol</t>
+  </si>
+  <si>
+    <t>Metroniazol</t>
+  </si>
+  <si>
+    <t>Nistatina</t>
+  </si>
+  <si>
+    <t>Augmentin</t>
+  </si>
+  <si>
+    <t>Erytromecina</t>
+  </si>
+  <si>
+    <t>added 16-02-2022</t>
+  </si>
+  <si>
+    <t>added 16-02-2023</t>
+  </si>
+  <si>
+    <t>added 16-02-2024</t>
+  </si>
+  <si>
+    <t>added 16-02-2025</t>
+  </si>
+  <si>
+    <t>added 16-02-2026</t>
+  </si>
+  <si>
+    <t>added 16-02-2027</t>
+  </si>
+  <si>
+    <t>added 16-02-2028</t>
+  </si>
+  <si>
+    <t>added 16-02-2029</t>
+  </si>
+  <si>
+    <t>added 16-02-2030</t>
+  </si>
+  <si>
+    <t>added 16-02-2031</t>
+  </si>
+  <si>
+    <t>added 16-02-2032</t>
+  </si>
+  <si>
+    <t>added 16-02-2033</t>
+  </si>
+  <si>
+    <t>changeregno</t>
+  </si>
+  <si>
+    <t>changeregdate</t>
+  </si>
+  <si>
+    <t>REGDATE</t>
+  </si>
+  <si>
+    <t>data('MOTCONT')=='1'</t>
+  </si>
+  <si>
+    <t>data("DATINC")</t>
+  </si>
+  <si>
+    <t>data("INTINICI")</t>
+  </si>
+  <si>
     <t>(data('ID')&gt;999999  &amp;&amp; data('ID')&lt;10000000) || data('BAIRRO') == 77</t>
   </si>
   <si>
-    <t>data('REGIDC') &gt; 99999999 &amp;&amp; data('REGIDC') &lt; 1000000000 || data('BAIRRO') != 77</t>
-  </si>
-  <si>
-    <t>data('CAMOONDE') != null || data('TABZ') == 7777 || data('CAMO') != 9999</t>
-  </si>
-  <si>
-    <t>data('CAMO') != null || data('CAMOONDE') != null</t>
-  </si>
-  <si>
-    <t>OBS</t>
-  </si>
-  <si>
-    <t>Abrao</t>
-  </si>
-  <si>
-    <t>Augosto Da Costa</t>
-  </si>
-  <si>
-    <t>Abdel</t>
-  </si>
-  <si>
-    <t>Fatima</t>
-  </si>
-  <si>
-    <t>TRATAMENT_A</t>
-  </si>
-  <si>
-    <t>A criança recebeu algum tratamento (antes inclusao)?</t>
-  </si>
-  <si>
-    <t>data('TRATAMENT_A') =='1'</t>
-  </si>
-  <si>
-    <t>TRATQUAL_A</t>
-  </si>
-  <si>
-    <t>TRATAMENT_R</t>
-  </si>
-  <si>
-    <t>Did the child get any treatments prescribed?</t>
-  </si>
-  <si>
-    <t>A criança deve receber algum tratamento (receita)?</t>
-  </si>
-  <si>
-    <t>TRATQUAL_R</t>
-  </si>
-  <si>
-    <t>What treatments are prescribed ?</t>
-  </si>
-  <si>
-    <t>Qual tratamento foi receitado?</t>
-  </si>
-  <si>
-    <t>TRATQUALOU_R</t>
-  </si>
-  <si>
-    <t>TRATQUALOU_A</t>
-  </si>
-  <si>
-    <t>selected(data('TRATQUAL_R'),'77')</t>
-  </si>
-  <si>
-    <t>data('TRATAMENT_R') =='1'</t>
-  </si>
-  <si>
-    <t>selected(data('TRATQUAL_A'),'77')</t>
-  </si>
-  <si>
-    <t>Paracetamol</t>
-  </si>
-  <si>
-    <t>Amoxicillina</t>
-  </si>
-  <si>
-    <t>Complexo B</t>
-  </si>
-  <si>
-    <t>Salbutamol</t>
-  </si>
-  <si>
-    <t>Diazepam</t>
-  </si>
-  <si>
-    <t>Prometazina</t>
-  </si>
-  <si>
-    <t>Treatment 7</t>
-  </si>
-  <si>
-    <t>Treatment 8</t>
-  </si>
-  <si>
-    <t>Tratamento 8</t>
-  </si>
-  <si>
-    <t>Tratamento 7</t>
-  </si>
-  <si>
-    <t>Treatment 9</t>
-  </si>
-  <si>
-    <t>Tratamento 9</t>
-  </si>
-  <si>
-    <t>Treatment 10</t>
-  </si>
-  <si>
-    <t>Tratamento 10</t>
-  </si>
-  <si>
-    <t>Treatment 11</t>
-  </si>
-  <si>
-    <t>Tratamento 11</t>
-  </si>
-  <si>
-    <t>Treatment 12</t>
-  </si>
-  <si>
-    <t>Tratamento 12</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>removed Suzete (enf=1) on 19-01-2022</t>
-  </si>
-  <si>
-    <t>removed Suzete (ass=11) on 19-01-2022</t>
+    <t>data('REGIDC') &gt; 10000000 &amp;&amp; data('REGIDC') &lt; 170000000 || data('BAIRRO') != 77</t>
+  </si>
+  <si>
+    <t>Deve ter 8 dígitos:</t>
+  </si>
+  <si>
+    <t>Must be 8 digits long:</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1569,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1525,6 +1585,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1553,7 +1619,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1574,6 +1640,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1971,7 +2038,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2030,11 +2097,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R221"/>
+  <dimension ref="A1:R226"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E146" sqref="E146"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2257,13 +2324,13 @@
         <v>413</v>
       </c>
       <c r="K14" t="s">
+        <v>419</v>
+      </c>
+      <c r="L14" t="s">
         <v>421</v>
       </c>
-      <c r="L14" t="s">
-        <v>423</v>
-      </c>
       <c r="M14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -2326,13 +2393,13 @@
         <v>309</v>
       </c>
       <c r="K19" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="L19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="M19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
@@ -2382,13 +2449,13 @@
         <v>260</v>
       </c>
       <c r="K23" t="s">
+        <v>419</v>
+      </c>
+      <c r="L23" t="s">
         <v>421</v>
       </c>
-      <c r="L23" t="s">
-        <v>423</v>
-      </c>
       <c r="M23" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -2668,8 +2735,8 @@
       <c r="H50" t="s">
         <v>190</v>
       </c>
-      <c r="K50" s="2" t="s">
-        <v>419</v>
+      <c r="K50" s="16" t="s">
+        <v>480</v>
       </c>
       <c r="L50" t="s">
         <v>270</v>
@@ -2737,13 +2804,13 @@
         <v>388</v>
       </c>
       <c r="K56" t="s">
-        <v>420</v>
+        <v>481</v>
       </c>
       <c r="L56" t="s">
-        <v>275</v>
+        <v>483</v>
       </c>
       <c r="M56" t="s">
-        <v>387</v>
+        <v>482</v>
       </c>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.35">
@@ -3437,18 +3504,20 @@
       </c>
     </row>
     <row r="117" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D117" t="s">
+      <c r="D117" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F117" t="s">
+      <c r="E117" s="2"/>
+      <c r="F117" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G117" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="H117" t="s">
+      <c r="H117" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="I117" s="2"/>
       <c r="K117" t="s">
         <v>230</v>
       </c>
@@ -3526,65 +3595,74 @@
       </c>
     </row>
     <row r="124" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B124" t="s">
-        <v>13</v>
-      </c>
+      <c r="B124" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C124" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="D124" s="18"/>
+      <c r="E124" s="18"/>
+      <c r="F124" s="18"/>
+      <c r="G124" s="18"/>
+      <c r="H124" s="18"/>
+      <c r="I124" s="18"/>
     </row>
     <row r="125" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B125" t="s">
-        <v>12</v>
+      <c r="B125" s="18"/>
+      <c r="C125" s="18"/>
+      <c r="D125" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E125" s="18"/>
+      <c r="F125" s="18" t="s">
+        <v>476</v>
+      </c>
+      <c r="G125" s="18"/>
+      <c r="H125" s="18"/>
+      <c r="I125" s="18" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D126" t="s">
-        <v>49</v>
-      </c>
-      <c r="E126" t="s">
-        <v>134</v>
-      </c>
-      <c r="F126" t="s">
-        <v>75</v>
-      </c>
-      <c r="G126" t="s">
-        <v>125</v>
-      </c>
-      <c r="H126" t="s">
-        <v>123</v>
-      </c>
+      <c r="B126" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C126" s="18"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="18"/>
+      <c r="H126" s="18"/>
+      <c r="I126" s="18"/>
     </row>
     <row r="127" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D127" t="s">
-        <v>49</v>
-      </c>
-      <c r="E127" t="s">
-        <v>134</v>
-      </c>
-      <c r="F127" t="s">
-        <v>382</v>
-      </c>
-      <c r="G127" t="s">
-        <v>124</v>
-      </c>
-      <c r="H127" t="s">
-        <v>76</v>
+      <c r="B127" s="18"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E127" s="18"/>
+      <c r="F127" s="18" t="s">
+        <v>476</v>
+      </c>
+      <c r="G127" s="18"/>
+      <c r="H127" s="18"/>
+      <c r="I127" s="18" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="128" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D128" t="s">
-        <v>49</v>
-      </c>
-      <c r="E128" t="s">
-        <v>134</v>
-      </c>
-      <c r="F128" t="s">
-        <v>77</v>
-      </c>
-      <c r="G128" t="s">
-        <v>126</v>
-      </c>
-      <c r="H128" t="s">
-        <v>127</v>
-      </c>
+      <c r="B128" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C128" s="18"/>
+      <c r="D128" s="18"/>
+      <c r="E128" s="18"/>
+      <c r="F128" s="18"/>
+      <c r="G128" s="18"/>
+      <c r="H128" s="18"/>
+      <c r="I128" s="18"/>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
@@ -3604,366 +3682,369 @@
         <v>134</v>
       </c>
       <c r="F131" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G131" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H131" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D132" t="s">
+        <v>49</v>
+      </c>
+      <c r="E132" t="s">
+        <v>134</v>
+      </c>
+      <c r="F132" t="s">
+        <v>382</v>
+      </c>
+      <c r="G132" t="s">
+        <v>124</v>
+      </c>
+      <c r="H132" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D133" t="s">
+        <v>49</v>
+      </c>
+      <c r="E133" t="s">
+        <v>134</v>
+      </c>
+      <c r="F133" t="s">
+        <v>77</v>
+      </c>
+      <c r="G133" t="s">
+        <v>126</v>
+      </c>
+      <c r="H133" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B135" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D136" t="s">
+        <v>49</v>
+      </c>
+      <c r="E136" t="s">
+        <v>134</v>
+      </c>
+      <c r="F136" t="s">
+        <v>78</v>
+      </c>
+      <c r="G136" t="s">
+        <v>128</v>
+      </c>
+      <c r="H136" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D137" t="s">
         <v>45</v>
       </c>
-      <c r="F132" t="s">
+      <c r="F137" t="s">
         <v>80</v>
       </c>
-      <c r="G132" t="s">
+      <c r="G137" t="s">
         <v>129</v>
       </c>
-      <c r="H132" t="s">
+      <c r="H137" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B133" t="s">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B138" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B134" s="17" t="s">
+    <row r="139" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B139" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D135" s="17" t="s">
+    <row r="140" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D140" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E135" s="17" t="s">
+      <c r="E140" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="F135" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="G135" s="17" t="s">
+      <c r="F140" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="G140" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="H135" s="17" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="136" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B136" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C136" s="17" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="137" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D137" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E137" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="F137" s="17" t="s">
-        <v>431</v>
-      </c>
-      <c r="G137" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="H137" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="138" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B138" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C138" s="17" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="139" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D139" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F139" s="17" t="s">
-        <v>439</v>
-      </c>
-      <c r="G139" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="H139" s="17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="140" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B140" s="17" t="s">
-        <v>58</v>
+      <c r="H140" s="17" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="141" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B141" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="C141" s="17" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="142" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B142" s="17" t="s">
-        <v>13</v>
+      <c r="D142" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E142" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="F142" s="17" t="s">
+        <v>429</v>
+      </c>
+      <c r="G142" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="H142" s="17" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="143" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B143" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C143" s="17" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="144" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D144" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F144" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="G144" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="H144" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B145" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B146" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B147" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D144" s="16" t="s">
+    <row r="149" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D149" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E144" s="16" t="s">
+      <c r="E149" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="F144" s="16" t="s">
+      <c r="F149" s="16" t="s">
+        <v>430</v>
+      </c>
+      <c r="G149" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="H149" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="G144" s="16" t="s">
+    </row>
+    <row r="150" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B150" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C150" s="16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D151" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E151" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="F151" s="16" t="s">
         <v>433</v>
       </c>
-      <c r="H144" s="16" t="s">
+      <c r="G151" s="16" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="145" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="16" t="s">
+      <c r="H151" s="16" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B152" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C145" s="16" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="146" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D146" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E146" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="F146" s="16" t="s">
-        <v>435</v>
-      </c>
-      <c r="G146" s="16" t="s">
+      <c r="C152" s="16" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D153" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F153" s="16" t="s">
         <v>436</v>
       </c>
-      <c r="H146" s="16" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="147" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="16" t="s">
+      <c r="G153" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="H153" s="16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B154" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B155" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="156" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B156" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B157" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D158" t="s">
+        <v>349</v>
+      </c>
+      <c r="F158" t="s">
+        <v>378</v>
+      </c>
+      <c r="G158" t="s">
+        <v>381</v>
+      </c>
+      <c r="H158" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B159" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B160" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D161" t="s">
+        <v>49</v>
+      </c>
+      <c r="E161" t="s">
+        <v>53</v>
+      </c>
+      <c r="F161" t="s">
+        <v>83</v>
+      </c>
+      <c r="G161" t="s">
+        <v>131</v>
+      </c>
+      <c r="H161" t="s">
+        <v>398</v>
+      </c>
+      <c r="K161" t="s">
+        <v>359</v>
+      </c>
+      <c r="L161" t="s">
+        <v>362</v>
+      </c>
+      <c r="M161" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="162" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B162" t="s">
         <v>56</v>
       </c>
-      <c r="C147" s="16" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="148" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D148" s="16" t="s">
+      <c r="C162" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="163" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D163" t="s">
         <v>45</v>
       </c>
-      <c r="F148" s="16" t="s">
-        <v>438</v>
-      </c>
-      <c r="G148" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="H148" s="16" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="149" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B149" s="16" t="s">
+      <c r="F163" t="s">
+        <v>84</v>
+      </c>
+      <c r="G163" t="s">
+        <v>130</v>
+      </c>
+      <c r="H163" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="164" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B164" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="151" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="152" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B152" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="153" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D153" t="s">
-        <v>349</v>
-      </c>
-      <c r="F153" t="s">
-        <v>378</v>
-      </c>
-      <c r="G153" t="s">
-        <v>381</v>
-      </c>
-      <c r="H153" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="154" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B154" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="155" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B155" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="156" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D156" t="s">
+    <row r="165" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D165" t="s">
         <v>49</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E165" t="s">
         <v>53</v>
       </c>
-      <c r="F156" t="s">
-        <v>83</v>
-      </c>
-      <c r="G156" t="s">
-        <v>131</v>
-      </c>
-      <c r="H156" t="s">
-        <v>398</v>
-      </c>
-      <c r="K156" t="s">
-        <v>359</v>
-      </c>
-      <c r="L156" t="s">
+      <c r="F165" t="s">
+        <v>96</v>
+      </c>
+      <c r="G165" t="s">
+        <v>132</v>
+      </c>
+      <c r="H165" t="s">
+        <v>399</v>
+      </c>
+      <c r="K165" t="s">
+        <v>360</v>
+      </c>
+      <c r="L165" t="s">
         <v>362</v>
       </c>
-      <c r="M156" t="s">
+      <c r="M165" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="157" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B157" t="s">
-        <v>56</v>
-      </c>
-      <c r="C157" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="158" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D158" t="s">
-        <v>45</v>
-      </c>
-      <c r="F158" t="s">
-        <v>84</v>
-      </c>
-      <c r="G158" t="s">
-        <v>130</v>
-      </c>
-      <c r="H158" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="159" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B159" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="160" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D160" t="s">
-        <v>49</v>
-      </c>
-      <c r="E160" t="s">
-        <v>53</v>
-      </c>
-      <c r="F160" t="s">
-        <v>96</v>
-      </c>
-      <c r="G160" t="s">
-        <v>132</v>
-      </c>
-      <c r="H160" t="s">
-        <v>399</v>
-      </c>
-      <c r="K160" t="s">
-        <v>360</v>
-      </c>
-      <c r="L160" t="s">
-        <v>362</v>
-      </c>
-      <c r="M160" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="161" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B161" t="s">
-        <v>56</v>
-      </c>
-      <c r="C161" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="162" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D162" t="s">
-        <v>45</v>
-      </c>
-      <c r="F162" t="s">
-        <v>143</v>
-      </c>
-      <c r="G162" t="s">
-        <v>130</v>
-      </c>
-      <c r="H162" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="163" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B163" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="164" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D164" t="s">
-        <v>49</v>
-      </c>
-      <c r="E164" t="s">
-        <v>134</v>
-      </c>
-      <c r="F164" t="s">
-        <v>343</v>
-      </c>
-      <c r="G164" t="s">
-        <v>344</v>
-      </c>
-      <c r="H164" t="s">
-        <v>345</v>
-      </c>
-      <c r="K164" t="s">
-        <v>361</v>
-      </c>
-      <c r="L164" t="s">
-        <v>362</v>
-      </c>
-      <c r="M164" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="165" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B165" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="166" spans="2:13" x14ac:dyDescent="0.35">
@@ -3971,319 +4052,334 @@
         <v>56</v>
       </c>
       <c r="C166" t="s">
-        <v>346</v>
+        <v>97</v>
       </c>
     </row>
     <row r="167" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B167" t="s">
-        <v>12</v>
+      <c r="D167" t="s">
+        <v>45</v>
+      </c>
+      <c r="F167" t="s">
+        <v>143</v>
+      </c>
+      <c r="G167" t="s">
+        <v>130</v>
+      </c>
+      <c r="H167" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="168" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D168" t="s">
-        <v>105</v>
-      </c>
-      <c r="F168" t="s">
-        <v>210</v>
-      </c>
-      <c r="I168">
-        <v>2</v>
+      <c r="B168" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="169" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D169" t="s">
-        <v>33</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>214</v>
+        <v>49</v>
+      </c>
+      <c r="E169" t="s">
+        <v>134</v>
+      </c>
+      <c r="F169" t="s">
+        <v>343</v>
+      </c>
+      <c r="G169" t="s">
+        <v>344</v>
       </c>
       <c r="H169" t="s">
-        <v>400</v>
+        <v>345</v>
+      </c>
+      <c r="K169" t="s">
+        <v>361</v>
+      </c>
+      <c r="L169" t="s">
+        <v>362</v>
+      </c>
+      <c r="M169" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="170" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="171" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B171" t="s">
         <v>56</v>
       </c>
-      <c r="C170" t="s">
-        <v>90</v>
-      </c>
-      <c r="G170" s="2"/>
-    </row>
-    <row r="171" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D171" t="s">
-        <v>33</v>
-      </c>
-      <c r="G171" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="H171" t="s">
-        <v>285</v>
+      <c r="C171" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="172" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
-        <v>58</v>
-      </c>
-      <c r="G172" s="2"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="173" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B173" t="s">
-        <v>56</v>
-      </c>
-      <c r="C173" t="s">
-        <v>97</v>
-      </c>
-      <c r="G173" s="2"/>
+      <c r="D173" t="s">
+        <v>105</v>
+      </c>
+      <c r="F173" t="s">
+        <v>210</v>
+      </c>
+      <c r="I173">
+        <v>2</v>
+      </c>
     </row>
     <row r="174" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D174" t="s">
         <v>33</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H174" t="s">
-        <v>233</v>
+        <v>400</v>
       </c>
     </row>
     <row r="175" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
+        <v>56</v>
+      </c>
+      <c r="C175" t="s">
+        <v>90</v>
+      </c>
+      <c r="G175" s="2"/>
+    </row>
+    <row r="176" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D176" t="s">
+        <v>33</v>
+      </c>
+      <c r="G176" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H176" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B177" t="s">
         <v>58</v>
       </c>
-      <c r="G175" s="2"/>
-    </row>
-    <row r="176" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B176" t="s">
-        <v>56</v>
-      </c>
-      <c r="C176" t="s">
-        <v>347</v>
-      </c>
-      <c r="G176" s="2"/>
-    </row>
-    <row r="177" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D177" t="s">
-        <v>33</v>
-      </c>
-      <c r="G177" t="s">
-        <v>348</v>
-      </c>
-      <c r="H177" t="s">
-        <v>401</v>
-      </c>
+      <c r="G177" s="2"/>
     </row>
     <row r="178" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
+        <v>56</v>
+      </c>
+      <c r="C178" t="s">
+        <v>97</v>
+      </c>
+      <c r="G178" s="2"/>
+    </row>
+    <row r="179" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D179" t="s">
+        <v>33</v>
+      </c>
+      <c r="G179" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H179" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B180" t="s">
         <v>58</v>
       </c>
-      <c r="G178" s="2"/>
-    </row>
-    <row r="179" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B179" t="s">
-        <v>56</v>
-      </c>
-      <c r="C179" t="s">
-        <v>211</v>
-      </c>
-      <c r="G179" s="2"/>
-    </row>
-    <row r="180" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D180" t="s">
-        <v>33</v>
-      </c>
-      <c r="G180" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H180" t="s">
-        <v>402</v>
-      </c>
+      <c r="G180" s="2"/>
     </row>
     <row r="181" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
+        <v>56</v>
+      </c>
+      <c r="C181" t="s">
+        <v>347</v>
+      </c>
+      <c r="G181" s="2"/>
+    </row>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D182" t="s">
+        <v>33</v>
+      </c>
+      <c r="G182" t="s">
+        <v>348</v>
+      </c>
+      <c r="H182" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B183" t="s">
         <v>58</v>
       </c>
-      <c r="G181" s="2"/>
-    </row>
-    <row r="182" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B182" t="s">
-        <v>56</v>
-      </c>
-      <c r="C182" t="s">
-        <v>213</v>
-      </c>
-      <c r="G182" s="2"/>
-    </row>
-    <row r="183" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D183" t="s">
-        <v>33</v>
-      </c>
-      <c r="G183" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="H183" t="s">
-        <v>403</v>
-      </c>
+      <c r="G183" s="2"/>
     </row>
     <row r="184" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
+        <v>56</v>
+      </c>
+      <c r="C184" t="s">
+        <v>211</v>
+      </c>
+      <c r="G184" s="2"/>
+    </row>
+    <row r="185" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D185" t="s">
+        <v>33</v>
+      </c>
+      <c r="G185" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H185" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="186" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B186" t="s">
         <v>58</v>
       </c>
-      <c r="G184" s="2"/>
-    </row>
-    <row r="185" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B185" t="s">
-        <v>56</v>
-      </c>
-      <c r="C185" t="s">
-        <v>215</v>
-      </c>
-      <c r="G185" s="2"/>
-    </row>
-    <row r="186" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D186" t="s">
-        <v>33</v>
-      </c>
-      <c r="G186" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H186" t="s">
-        <v>234</v>
-      </c>
+      <c r="G186" s="2"/>
     </row>
     <row r="187" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
+        <v>56</v>
+      </c>
+      <c r="C187" t="s">
+        <v>213</v>
+      </c>
+      <c r="G187" s="2"/>
+    </row>
+    <row r="188" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D188" t="s">
+        <v>33</v>
+      </c>
+      <c r="G188" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H188" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B189" t="s">
         <v>58</v>
       </c>
-      <c r="G187" s="2"/>
-    </row>
-    <row r="188" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B188" t="s">
-        <v>56</v>
-      </c>
-      <c r="C188" t="s">
-        <v>217</v>
-      </c>
-      <c r="G188" s="2"/>
-    </row>
-    <row r="189" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D189" t="s">
-        <v>33</v>
-      </c>
-      <c r="G189" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="H189" t="s">
-        <v>199</v>
-      </c>
+      <c r="G189" s="2"/>
     </row>
     <row r="190" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
-        <v>58</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C190" t="s">
+        <v>215</v>
+      </c>
+      <c r="G190" s="2"/>
     </row>
     <row r="191" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B191" t="s">
-        <v>13</v>
+      <c r="D191" t="s">
+        <v>33</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H191" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="192" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
-        <v>169</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="G192" s="2"/>
     </row>
     <row r="193" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B193" t="s">
-        <v>12</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C193" t="s">
+        <v>217</v>
+      </c>
+      <c r="G193" s="2"/>
     </row>
     <row r="194" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D194" t="s">
+        <v>33</v>
+      </c>
+      <c r="G194" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="H194" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="195" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B195" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="196" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B196" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B197" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="198" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B198" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="199" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="D199" t="s">
         <v>39</v>
       </c>
-      <c r="F194" s="2" t="s">
+      <c r="F199" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G194" s="2" t="s">
+      <c r="G199" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H194" t="s">
+      <c r="H199" t="s">
         <v>193</v>
       </c>
-      <c r="K194" s="2" t="s">
+      <c r="K199" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="L194" t="s">
+      <c r="L199" t="s">
         <v>293</v>
       </c>
-      <c r="M194" t="s">
+      <c r="M199" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="195" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="D195" t="s">
+    <row r="200" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="D200" t="s">
         <v>39</v>
       </c>
-      <c r="F195" s="2" t="s">
+      <c r="F200" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G195" s="2" t="s">
+      <c r="G200" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="H195" t="s">
+      <c r="H200" t="s">
         <v>194</v>
       </c>
-      <c r="K195" t="s">
+      <c r="K200" t="s">
         <v>219</v>
       </c>
-      <c r="L195" t="s">
+      <c r="L200" t="s">
         <v>294</v>
       </c>
-      <c r="M195" t="s">
+      <c r="M200" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="196" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="D196" t="s">
-        <v>105</v>
-      </c>
-      <c r="F196" t="s">
-        <v>299</v>
-      </c>
-      <c r="I196" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="197" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="D197" t="s">
-        <v>33</v>
-      </c>
-      <c r="G197" t="s">
-        <v>301</v>
-      </c>
-      <c r="H197" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="198" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="D198" t="s">
-        <v>105</v>
-      </c>
-      <c r="F198" t="s">
-        <v>210</v>
-      </c>
-      <c r="I198">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B199" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="200" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B200" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="201" spans="2:17" x14ac:dyDescent="0.35">
@@ -4291,84 +4387,42 @@
         <v>105</v>
       </c>
       <c r="F201" t="s">
-        <v>85</v>
+        <v>299</v>
       </c>
       <c r="I201" t="s">
-        <v>186</v>
+        <v>300</v>
       </c>
     </row>
     <row r="202" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D202" t="s">
-        <v>31</v>
-      </c>
-      <c r="F202" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="G202" t="s">
-        <v>139</v>
+        <v>301</v>
       </c>
       <c r="H202" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q202" t="b">
-        <v>0</v>
+        <v>302</v>
       </c>
     </row>
     <row r="203" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D203" t="s">
-        <v>226</v>
+        <v>105</v>
       </c>
       <c r="F203" t="s">
-        <v>373</v>
-      </c>
-      <c r="G203" t="s">
-        <v>209</v>
-      </c>
-      <c r="H203" t="s">
-        <v>140</v>
-      </c>
-      <c r="K203" t="s">
-        <v>377</v>
-      </c>
-      <c r="L203" t="s">
-        <v>362</v>
-      </c>
-      <c r="M203" t="s">
-        <v>363</v>
+        <v>210</v>
+      </c>
+      <c r="I203">
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="D204" t="s">
-        <v>105</v>
-      </c>
-      <c r="F204" t="s">
-        <v>86</v>
-      </c>
-      <c r="I204" t="s">
-        <v>376</v>
+      <c r="B204" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="205" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="D205" t="s">
-        <v>39</v>
-      </c>
-      <c r="F205" t="s">
-        <v>372</v>
-      </c>
-      <c r="G205" t="s">
-        <v>109</v>
-      </c>
-      <c r="H205" t="s">
-        <v>110</v>
-      </c>
-      <c r="K205" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="L205" t="s">
-        <v>295</v>
-      </c>
-      <c r="M205" t="s">
-        <v>298</v>
+      <c r="B205" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="206" spans="2:17" x14ac:dyDescent="0.35">
@@ -4376,133 +4430,218 @@
         <v>105</v>
       </c>
       <c r="F206" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="I206" t="s">
-        <v>375</v>
+        <v>186</v>
       </c>
     </row>
     <row r="207" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D207" t="s">
+        <v>31</v>
+      </c>
+      <c r="F207" t="s">
+        <v>85</v>
+      </c>
+      <c r="G207" t="s">
+        <v>139</v>
+      </c>
+      <c r="H207" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q207" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="D208" t="s">
+        <v>226</v>
+      </c>
+      <c r="F208" t="s">
+        <v>373</v>
+      </c>
+      <c r="G208" t="s">
+        <v>209</v>
+      </c>
+      <c r="H208" t="s">
+        <v>140</v>
+      </c>
+      <c r="K208" t="s">
+        <v>377</v>
+      </c>
+      <c r="L208" t="s">
+        <v>362</v>
+      </c>
+      <c r="M208" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="209" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D209" t="s">
+        <v>105</v>
+      </c>
+      <c r="F209" t="s">
+        <v>86</v>
+      </c>
+      <c r="I209" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="210" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D210" t="s">
+        <v>39</v>
+      </c>
+      <c r="F210" t="s">
+        <v>372</v>
+      </c>
+      <c r="G210" t="s">
+        <v>109</v>
+      </c>
+      <c r="H210" t="s">
+        <v>110</v>
+      </c>
+      <c r="K210" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="L210" t="s">
+        <v>295</v>
+      </c>
+      <c r="M210" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="211" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D211" t="s">
+        <v>105</v>
+      </c>
+      <c r="F211" t="s">
+        <v>40</v>
+      </c>
+      <c r="I211" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="212" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D212" t="s">
         <v>33</v>
       </c>
-      <c r="G207" t="s">
+      <c r="G212" t="s">
         <v>311</v>
       </c>
-      <c r="H207" t="s">
+      <c r="H212" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="208" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B208" t="s">
+    <row r="213" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B213" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="209" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B209" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B210" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="211" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D211" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E211" t="s">
-        <v>195</v>
-      </c>
-      <c r="F211" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G211" t="s">
-        <v>141</v>
-      </c>
-      <c r="H211" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="212" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B212" t="s">
-        <v>56</v>
-      </c>
-      <c r="C212" t="s">
-        <v>220</v>
-      </c>
-      <c r="D212" s="2"/>
-      <c r="F212" s="2"/>
-    </row>
-    <row r="213" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D213" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E213" t="s">
-        <v>196</v>
-      </c>
-      <c r="F213" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G213" t="s">
-        <v>142</v>
-      </c>
-      <c r="H213" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="214" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B214" t="s">
         <v>58</v>
       </c>
-      <c r="D214" s="2"/>
-      <c r="F214" s="2"/>
-    </row>
-    <row r="215" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="215" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B215" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="216" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B216" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="217" spans="2:9" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="216" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D216" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E216" t="s">
+        <v>195</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G216" t="s">
+        <v>141</v>
+      </c>
+      <c r="H216" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="217" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B217" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="218" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D218" t="s">
-        <v>33</v>
+        <v>56</v>
+      </c>
+      <c r="C217" t="s">
+        <v>220</v>
+      </c>
+      <c r="D217" s="2"/>
+      <c r="F217" s="2"/>
+    </row>
+    <row r="218" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D218" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E218" t="s">
+        <v>196</v>
+      </c>
+      <c r="F218" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="G218" t="s">
-        <v>205</v>
+        <v>142</v>
       </c>
       <c r="H218" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="219" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D219" t="s">
-        <v>105</v>
-      </c>
-      <c r="F219" t="s">
-        <v>210</v>
-      </c>
-      <c r="I219">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="219" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B219" t="s">
+        <v>58</v>
+      </c>
+      <c r="D219" s="2"/>
+      <c r="F219" s="2"/>
+    </row>
+    <row r="220" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B220" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="221" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B221" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="222" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B222" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="223" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D223" t="s">
+        <v>33</v>
+      </c>
+      <c r="G223" t="s">
+        <v>205</v>
+      </c>
+      <c r="H223" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="224" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="D224" t="s">
+        <v>105</v>
+      </c>
+      <c r="F224" t="s">
+        <v>210</v>
+      </c>
+      <c r="I224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B225" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B226" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4514,11 +4653,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A20:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4543,7 +4682,7 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -4719,13 +4858,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -4737,10 +4876,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -4752,10 +4891,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -4767,16 +4906,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>196</v>
       </c>
@@ -4785,13 +4924,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>196</v>
       </c>
@@ -4800,13 +4939,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>196</v>
       </c>
@@ -4815,13 +4954,13 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>207</v>
       </c>
@@ -4830,13 +4969,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>207</v>
       </c>
@@ -4845,13 +4984,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>207</v>
       </c>
@@ -4860,13 +4999,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>207</v>
       </c>
@@ -4875,13 +5014,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>207</v>
       </c>
@@ -4890,13 +5029,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>207</v>
       </c>
@@ -4905,13 +5044,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>207</v>
       </c>
@@ -4920,13 +5059,16 @@
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>450</v>
+      </c>
+      <c r="E26" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -4935,13 +5077,16 @@
         <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>207</v>
       </c>
@@ -4950,13 +5095,16 @@
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+      <c r="E28" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>207</v>
       </c>
@@ -4965,13 +5113,16 @@
         <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>453</v>
+      </c>
+      <c r="E29" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>207</v>
       </c>
@@ -4980,13 +5131,16 @@
         <v>11</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>454</v>
+      </c>
+      <c r="E30" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>207</v>
       </c>
@@ -4995,271 +5149,364 @@
         <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>455</v>
+      </c>
+      <c r="E31" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>207</v>
       </c>
       <c r="B32" t="str">
+        <f>"13"</f>
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E32" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" t="str">
+        <f>"14"</f>
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E33" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" t="str">
+        <f>"15"</f>
+        <v>15</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E34" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" t="str">
+        <f>"16"</f>
+        <v>16</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E35" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" t="str">
+        <f>"17"</f>
+        <v>17</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="E36" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" t="str">
+        <f>"18"</f>
+        <v>18</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="E37" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" t="str">
         <f>"77"</f>
         <v>77</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>286</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B39" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>286</v>
       </c>
-      <c r="B34" s="2" t="str">
+      <c r="B40" s="2" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>287</v>
       </c>
-      <c r="B35" t="str">
+      <c r="B41" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>287</v>
       </c>
-      <c r="B36" s="2" t="str">
+      <c r="B42" s="2" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>287</v>
       </c>
-      <c r="B37" s="2" t="str">
+      <c r="B43" s="2" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>250</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B44" t="str">
         <f>"99"</f>
         <v>99</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D44" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B39" t="str">
+      <c r="B45" t="str">
         <f>"99"</f>
         <v>99</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>324</v>
-      </c>
-      <c r="B40" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>325</v>
-      </c>
-      <c r="D40" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>324</v>
-      </c>
-      <c r="B41" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>327</v>
-      </c>
-      <c r="D41" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>337</v>
-      </c>
-      <c r="B42" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>239</v>
-      </c>
-      <c r="D42" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>337</v>
-      </c>
-      <c r="B43" s="2" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>240</v>
-      </c>
-      <c r="D43" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>337</v>
-      </c>
-      <c r="B44" s="2" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>340</v>
-      </c>
-      <c r="D44" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>337</v>
-      </c>
-      <c r="B45" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C45" t="s">
-        <v>338</v>
-      </c>
-      <c r="D45" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>368</v>
       </c>
       <c r="B46" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C46" t="s">
+        <v>325</v>
+      </c>
+      <c r="D46" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>324</v>
+      </c>
+      <c r="B47" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>327</v>
+      </c>
+      <c r="D47" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>337</v>
+      </c>
+      <c r="B48" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>239</v>
+      </c>
+      <c r="D48" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>337</v>
+      </c>
+      <c r="B49" s="2" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>240</v>
+      </c>
+      <c r="D49" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>337</v>
+      </c>
+      <c r="B50" s="2" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>340</v>
+      </c>
+      <c r="D50" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>337</v>
+      </c>
+      <c r="B51" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>338</v>
+      </c>
+      <c r="D51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>368</v>
+      </c>
+      <c r="B52" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
         <v>162</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D52" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="4"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="4"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="4"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="4"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -5273,25 +5520,25 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
-      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="4"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B70" s="9"/>
+      <c r="A70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B71" s="9"/>
+      <c r="A71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B72" s="9"/>
+      <c r="A72" s="4"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B73" s="9"/>
+      <c r="A73" s="4"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B74" s="9"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B75" s="9"/>
+      <c r="A74" s="4"/>
+      <c r="D74" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B76" s="9"/>
@@ -5370,33 +5617,28 @@
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103" s="9"/>
-      <c r="C103" s="9"/>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" s="9"/>
-      <c r="C104" s="9"/>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105" s="9"/>
-      <c r="C105" s="9"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106" s="9"/>
-      <c r="C106" s="9"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B108" s="9"/>
       <c r="C108" s="9"/>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
@@ -5420,7 +5662,6 @@
       <c r="C113" s="9"/>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B114" s="9"/>
       <c r="C114" s="9"/>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
@@ -5473,53 +5714,59 @@
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B128" s="9"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C128" s="9"/>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B129" s="9"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C129" s="9"/>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B130" s="9"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C130" s="9"/>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B131" s="9"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C131" s="9"/>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B132" s="9"/>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C132" s="9"/>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B133" s="9"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B134" s="9"/>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B135" s="9"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B136" s="9"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B137" s="9"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B138" s="9"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B139" s="9"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B140" s="9"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B141" s="9"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B142" s="9"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B143" s="9"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B144" s="9"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.35">
@@ -5545,6 +5792,24 @@
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B152" s="9"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B153" s="9"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B154" s="9"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B155" s="9"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B156" s="9"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B157" s="9"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B158" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -5702,8 +5967,8 @@
   <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6448,7 +6713,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B67" t="s">
         <v>49</v>
@@ -6459,7 +6724,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B68" t="s">
         <v>49</v>
@@ -6492,7 +6757,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B71" t="s">
         <v>144</v>
@@ -6503,7 +6768,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B72" t="s">
         <v>144</v>
@@ -6525,7 +6790,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B74" t="s">
         <v>45</v>
@@ -6536,7 +6801,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B75" t="s">
         <v>45</v>
@@ -6595,52 +6860,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" s="8"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="8"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="8"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>474</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>475</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>476</v>
+      </c>
+      <c r="B83" t="s">
+        <v>31</v>
+      </c>
+      <c r="C83" t="b">
+        <v>0</v>
+      </c>
+      <c r="D83" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B84" s="8"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B85" s="8"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B86" s="8"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B87" s="8"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B88" s="8"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B89" s="8"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B91" s="8"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B92" s="8"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B93" s="8"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B94" s="8"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B95" s="8"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B96" s="8"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>